<commit_message>
Clean up problem NTD data.
</commit_message>
<xml_diff>
--- a/Factors and Ridership Data/Model Estimation/Est10/TNC Effect Charts.xlsx
+++ b/Factors and Ridership Data/Model Estimation/Est10/TNC Effect Charts.xlsx
@@ -1,18 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3101A967-6D1B-443F-AAA9-A3210D74025E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -66,9 +75,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -121,7 +130,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -180,7 +189,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -598,7 +606,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1016,7 +1023,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1424,7 +1430,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1632,102 +1637,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-AB45-4BA3-9AA4-684B57F2F22F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$D$35</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>UBER_REV_SCALED_SF</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$A$36:$A$44</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>2010</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2011</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2012</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2013</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2014</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2015</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2016</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2017</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2018</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$D$36:$D$44</c:f>
-              <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-8.3499999999999997E-5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-5.7336666666666606E-4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-2.4771666666666609E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-9.4076666666666111E-3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-2.7632933333333304E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-4.4154799999999994E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-6.2736333333333311E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-AB45-4BA3-9AA4-684B57F2F22F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1935,7 +1844,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2143,102 +2051,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-606C-4729-A662-01F014B465B2}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$J$35</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>UBER_REV_SCALED_LEX</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$G$36:$G$44</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>2010</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2011</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2012</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2013</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2014</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2015</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2016</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2017</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2018</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$J$36:$J$44</c:f>
-              <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-1.9E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-7.2157303370786437E-3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-2.1194606741572877E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-3.3866966292134648E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-4.8119101123595479E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-606C-4729-A662-01F014B465B2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2434,7 +2246,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2464,7 +2282,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -2496,7 +2320,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -2516,19 +2346,25 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>46</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1390651</xdr:colOff>
       <xdr:row>62</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -2547,20 +2383,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1422400</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>311150</xdr:colOff>
       <xdr:row>62</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -2842,26 +2684,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="B44" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.81640625" customWidth="1"/>
+    <col min="7" max="7" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.54296875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2869,7 +2711,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2892,7 +2734,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2010</v>
       </c>
@@ -2919,7 +2761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2011</v>
       </c>
@@ -2946,7 +2788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2012</v>
       </c>
@@ -2973,7 +2815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2013</v>
       </c>
@@ -3000,7 +2842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2014</v>
       </c>
@@ -3027,7 +2869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2015</v>
       </c>
@@ -3054,7 +2896,7 @@
         <v>3.79775280898876</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2016</v>
       </c>
@@ -3081,7 +2923,7 @@
         <v>11.155056179775199</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2017</v>
       </c>
@@ -3108,7 +2950,7 @@
         <v>17.824719101123499</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2018</v>
       </c>
@@ -3135,7 +2977,7 @@
         <v>25.325842696629199</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>10</v>
       </c>
@@ -3143,11 +2985,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
       <c r="G33" s="1"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>11</v>
       </c>
@@ -3177,7 +3019,7 @@
         <v>-1.9E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -3203,7 +3045,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>2010</v>
       </c>
@@ -3239,7 +3081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>2011</v>
       </c>
@@ -3252,7 +3094,7 @@
         <v>0</v>
       </c>
       <c r="D37" s="3">
-        <f t="shared" ref="D37:E37" si="3">D$34*D5</f>
+        <f t="shared" ref="D37" si="3">D$34*D5</f>
         <v>0</v>
       </c>
       <c r="E37" s="5">
@@ -3275,7 +3117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>2012</v>
       </c>
@@ -3288,7 +3130,7 @@
         <v>-1.9845E-4</v>
       </c>
       <c r="D38" s="3">
-        <f t="shared" ref="D38:E38" si="6">D$34*D6</f>
+        <f t="shared" ref="D38" si="6">D$34*D6</f>
         <v>-8.3499999999999997E-5</v>
       </c>
       <c r="E38" s="5">
@@ -3311,7 +3153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>2013</v>
       </c>
@@ -3324,7 +3166,7 @@
         <v>-1.36269E-3</v>
       </c>
       <c r="D39" s="3">
-        <f t="shared" ref="D39:E39" si="7">D$34*D7</f>
+        <f t="shared" ref="D39" si="7">D$34*D7</f>
         <v>-5.7336666666666606E-4</v>
       </c>
       <c r="E39" s="5">
@@ -3347,7 +3189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>2014</v>
       </c>
@@ -3360,7 +3202,7 @@
         <v>-5.8873500000000004E-3</v>
       </c>
       <c r="D40" s="3">
-        <f t="shared" ref="D40:E40" si="8">D$34*D8</f>
+        <f t="shared" ref="D40" si="8">D$34*D8</f>
         <v>-2.4771666666666609E-3</v>
       </c>
       <c r="E40" s="5">
@@ -3383,7 +3225,7 @@
         <v>-1.9E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>2015</v>
       </c>
@@ -3396,7 +3238,7 @@
         <v>-2.2358700000000002E-2</v>
       </c>
       <c r="D41" s="3">
-        <f t="shared" ref="D41:E41" si="9">D$34*D9</f>
+        <f t="shared" ref="D41" si="9">D$34*D9</f>
         <v>-9.4076666666666111E-3</v>
       </c>
       <c r="E41" s="5">
@@ -3419,7 +3261,7 @@
         <v>-7.2157303370786437E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>2016</v>
       </c>
@@ -3432,7 +3274,7 @@
         <v>-6.5673720000000005E-2</v>
       </c>
       <c r="D42" s="3">
-        <f t="shared" ref="D42:E42" si="10">D$34*D10</f>
+        <f t="shared" ref="D42" si="10">D$34*D10</f>
         <v>-2.7632933333333304E-2</v>
       </c>
       <c r="E42" s="5">
@@ -3455,7 +3297,7 @@
         <v>-2.1194606741572877E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>2017</v>
       </c>
@@ -3468,7 +3310,7 @@
         <v>-0.10494036</v>
       </c>
       <c r="D43" s="3">
-        <f t="shared" ref="D43:E43" si="11">D$34*D11</f>
+        <f t="shared" ref="D43" si="11">D$34*D11</f>
         <v>-4.4154799999999994E-2</v>
       </c>
       <c r="E43" s="5">
@@ -3491,7 +3333,7 @@
         <v>-3.3866966292134648E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>2018</v>
       </c>
@@ -3504,7 +3346,7 @@
         <v>-0.14910210000000002</v>
       </c>
       <c r="D44" s="3">
-        <f t="shared" ref="D44:E44" si="12">D$34*D12</f>
+        <f t="shared" ref="D44" si="12">D$34*D12</f>
         <v>-6.2736333333333311E-2</v>
       </c>
       <c r="E44" s="5">

</xml_diff>